<commit_message>
Add JS executable detection
</commit_message>
<xml_diff>
--- a/data/level1_analysis.xlsx
+++ b/data/level1_analysis.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,11 +461,7 @@
           <t>bot1</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>test111</t>
-        </is>
-      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="b">
         <v>1</v>
       </c>
@@ -481,11 +477,7 @@
           <t>guest</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>bot1</t>
-        </is>
-      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="b">
         <v>1</v>
       </c>
@@ -581,11 +573,7 @@
           <t>bot02</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>bot1</t>
-        </is>
-      </c>
+      <c r="B9" t="inlineStr"/>
       <c r="C9" t="b">
         <v>1</v>
       </c>
@@ -633,11 +621,7 @@
           <t>guest</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>bot02</t>
-        </is>
-      </c>
+      <c r="B12" t="inlineStr"/>
       <c r="C12" t="b">
         <v>1</v>
       </c>
@@ -669,11 +653,7 @@
           <t>guest</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>bot02</t>
-        </is>
-      </c>
+      <c r="B14" t="inlineStr"/>
       <c r="C14" t="b">
         <v>1</v>
       </c>
@@ -689,11 +669,7 @@
           <t>bot03</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>bottest01</t>
-        </is>
-      </c>
+      <c r="B15" t="inlineStr"/>
       <c r="C15" t="b">
         <v>1</v>
       </c>
@@ -709,17 +685,1821 @@
           <t>guest</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>bot03</t>
-        </is>
-      </c>
+      <c r="B16" t="inlineStr"/>
       <c r="C16" t="b">
         <v>0</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
           <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>webdriver=true; no plugins; UA contains Chrome but chrome flags missing; no mimeTypes</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>webdriver=true; no plugins; UA contains Chrome but chrome flags missing; no mimeTypes</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>webdriver=true; no plugins; UA contains Chrome but chrome flags missing; no mimeTypes</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>webdriver=true; no plugins; no mimeTypes</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>bot06</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing; outerVsScreenWidth suspicious=-270</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing; outerVsScreenWidth suspicious=-270</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>bot03</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="b">
+        <v>1</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>bot03</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="b">
+        <v>1</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>bot02</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="b">
+        <v>1</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>no plugins; UA contains Chrome but chrome flags missing; no mimeTypes</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr"/>
+      <c r="C32" t="b">
+        <v>1</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>no plugins; UA contains Chrome but chrome flags missing; no mimeTypes</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>bottest01</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="b">
+        <v>1</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>bottest01</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr"/>
+      <c r="C34" t="b">
+        <v>1</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>bottest01</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr"/>
+      <c r="C35" t="b">
+        <v>1</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr"/>
+      <c r="C36" t="b">
+        <v>1</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>bottest01</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr"/>
+      <c r="C37" t="b">
+        <v>1</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr"/>
+      <c r="C38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr"/>
+      <c r="C39" t="b">
+        <v>1</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr"/>
+      <c r="C40" t="b">
+        <v>1</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr"/>
+      <c r="C41" t="b">
+        <v>1</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr"/>
+      <c r="C42" t="b">
+        <v>1</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr"/>
+      <c r="C43" t="b">
+        <v>1</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr"/>
+      <c r="C44" t="b">
+        <v>1</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr"/>
+      <c r="C45" t="b">
+        <v>1</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>bot08</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr"/>
+      <c r="C46" t="b">
+        <v>1</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr"/>
+      <c r="C47" t="b">
+        <v>1</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>bot08</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr"/>
+      <c r="C48" t="b">
+        <v>1</v>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing; outerVsScreenWidth suspicious=-270</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr"/>
+      <c r="C49" t="b">
+        <v>1</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing; outerVsScreenWidth suspicious=-1470</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>bot05</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr"/>
+      <c r="C50" t="b">
+        <v>1</v>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>bot05</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr"/>
+      <c r="C51" t="b">
+        <v>1</v>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr"/>
+      <c r="C52" t="b">
+        <v>1</v>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>bot04</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr"/>
+      <c r="C53" t="b">
+        <v>1</v>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr"/>
+      <c r="C54" t="b">
+        <v>1</v>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>bot04</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr"/>
+      <c r="C55" t="b">
+        <v>1</v>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>bot04</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr"/>
+      <c r="C56" t="b">
+        <v>1</v>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr"/>
+      <c r="C57" t="b">
+        <v>1</v>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr"/>
+      <c r="C58" t="b">
+        <v>1</v>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr"/>
+      <c r="C59" t="b">
+        <v>1</v>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr"/>
+      <c r="C60" t="b">
+        <v>1</v>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr"/>
+      <c r="C61" t="b">
+        <v>1</v>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr"/>
+      <c r="C62" t="b">
+        <v>1</v>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing; outerVsScreenWidth suspicious=-1707</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>bottest01</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr"/>
+      <c r="C63" t="b">
+        <v>1</v>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>bottest01</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr"/>
+      <c r="C64" t="b">
+        <v>1</v>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>bottest01</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr"/>
+      <c r="C65" t="b">
+        <v>1</v>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr"/>
+      <c r="C66" t="b">
+        <v>1</v>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>bottest01</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr"/>
+      <c r="C67" t="b">
+        <v>1</v>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>bot04</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr"/>
+      <c r="C68" t="b">
+        <v>1</v>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>bot04</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr"/>
+      <c r="C69" t="b">
+        <v>1</v>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>bot04</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr"/>
+      <c r="C70" t="b">
+        <v>1</v>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr"/>
+      <c r="C71" t="b">
+        <v>1</v>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr"/>
+      <c r="C72" t="b">
+        <v>1</v>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr"/>
+      <c r="C73" t="b">
+        <v>1</v>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr"/>
+      <c r="C74" t="b">
+        <v>1</v>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr"/>
+      <c r="C75" t="b">
+        <v>1</v>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr"/>
+      <c r="C76" t="b">
+        <v>1</v>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr"/>
+      <c r="C77" t="b">
+        <v>1</v>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr"/>
+      <c r="C78" t="b">
+        <v>1</v>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr"/>
+      <c r="C79" t="b">
+        <v>1</v>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>bot08</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr"/>
+      <c r="C80" t="b">
+        <v>1</v>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>outerVsScreenWidth suspicious=-270</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr"/>
+      <c r="C81" t="b">
+        <v>1</v>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>outerVsScreenWidth suspicious=-270</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>bot08</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr"/>
+      <c r="C82" t="b">
+        <v>1</v>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>outerVsScreenWidth suspicious=-270</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr"/>
+      <c r="C83" t="b">
+        <v>1</v>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>outerVsScreenWidth suspicious=-270</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr"/>
+      <c r="C84" t="b">
+        <v>1</v>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr"/>
+      <c r="C85" t="b">
+        <v>1</v>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr"/>
+      <c r="C86" t="b">
+        <v>1</v>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr"/>
+      <c r="C87" t="b">
+        <v>1</v>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr"/>
+      <c r="C88" t="b">
+        <v>1</v>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr"/>
+      <c r="C89" t="b">
+        <v>1</v>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing; outerVsScreenWidth suspicious=-1707</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr"/>
+      <c r="C90" t="b">
+        <v>1</v>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr"/>
+      <c r="C91" t="b">
+        <v>1</v>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr"/>
+      <c r="C92" t="b">
+        <v>1</v>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr"/>
+      <c r="C93" t="b">
+        <v>1</v>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr"/>
+      <c r="C94" t="b">
+        <v>1</v>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing; outerVsScreenWidth suspicious=-1707</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr"/>
+      <c r="C95" t="b">
+        <v>1</v>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr"/>
+      <c r="C96" t="b">
+        <v>0</v>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr"/>
+      <c r="C97" t="b">
+        <v>0</v>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>bottest01</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr"/>
+      <c r="C98" t="b">
+        <v>1</v>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr"/>
+      <c r="C99" t="b">
+        <v>1</v>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>bot09</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr"/>
+      <c r="C100" t="b">
+        <v>1</v>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>webdriver=true; no plugins; UA contains Chrome but chrome flags missing; no mimeTypes; outerVsScreenWidth suspicious=224</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>bot09</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr"/>
+      <c r="C101" t="b">
+        <v>1</v>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>webdriver=true; no plugins; UA contains Chrome but chrome flags missing; no mimeTypes; outerVsScreenWidth suspicious=224</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>bot09</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr"/>
+      <c r="C102" t="b">
+        <v>1</v>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>bot09</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr"/>
+      <c r="C103" t="b">
+        <v>1</v>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>bot09</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr"/>
+      <c r="C104" t="b">
+        <v>1</v>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>bot09</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr"/>
+      <c r="C105" t="b">
+        <v>1</v>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>bot09</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr"/>
+      <c r="C106" t="b">
+        <v>1</v>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr"/>
+      <c r="C107" t="b">
+        <v>1</v>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr"/>
+      <c r="C108" t="b">
+        <v>1</v>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>bot09</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr"/>
+      <c r="C109" t="b">
+        <v>1</v>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr"/>
+      <c r="C110" t="b">
+        <v>1</v>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>bot09</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr"/>
+      <c r="C111" t="b">
+        <v>1</v>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>webdriver=true; no plugins; UA contains Chrome but chrome flags missing; no mimeTypes; outerVsScreenWidth suspicious=224</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>bot09</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr"/>
+      <c r="C112" t="b">
+        <v>1</v>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>webdriver=true; no plugins; UA contains Chrome but chrome flags missing; no mimeTypes; outerVsScreenWidth suspicious=224</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr"/>
+      <c r="C113" t="b">
+        <v>1</v>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>webdriver=true; no plugins; UA contains Chrome but chrome flags missing; no mimeTypes; outerVsScreenWidth suspicious=224</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr"/>
+      <c r="C114" t="b">
+        <v>1</v>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr"/>
+      <c r="C115" t="b">
+        <v>0</v>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>bot05</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr"/>
+      <c r="C116" t="b">
+        <v>1</v>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>webdriver=true; UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>bot05</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr"/>
+      <c r="C117" t="b">
+        <v>1</v>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>webdriver=true; UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr"/>
+      <c r="C118" t="b">
+        <v>1</v>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>webdriver=true; UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>bot05</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr"/>
+      <c r="C119" t="b">
+        <v>1</v>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>webdriver=true; UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>bot05</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr"/>
+      <c r="C120" t="b">
+        <v>1</v>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>webdriver=true; UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr"/>
+      <c r="C121" t="b">
+        <v>1</v>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>webdriver=true; UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>bot05</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr"/>
+      <c r="C122" t="b">
+        <v>1</v>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>webdriver=true; UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr"/>
+      <c r="C123" t="b">
+        <v>1</v>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>webdriver=true; UA contains Chrome but chrome flags missing</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>m.ik.k.am.u.e.rtio@gmail.com</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr"/>
+      <c r="C124" t="b">
+        <v>1</v>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>no plugins; UA contains Chrome but chrome flags missing; no mimeTypes</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>m.ik.k.am.u.e.rtio@gmail.com</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr"/>
+      <c r="C125" t="b">
+        <v>1</v>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>no plugins; UA contains Chrome but chrome flags missing; no mimeTypes</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr"/>
+      <c r="C126" t="b">
+        <v>1</v>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>no plugins; UA contains Chrome but chrome flags missing; no mimeTypes</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr"/>
+      <c r="C127" t="b">
+        <v>1</v>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>no plugins; UA contains Chrome but chrome flags missing; no mimeTypes</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr"/>
+      <c r="C128" t="b">
+        <v>1</v>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>no plugins; UA contains Chrome but chrome flags missing; no mimeTypes</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr"/>
+      <c r="C129" t="b">
+        <v>1</v>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>no plugins; UA contains Chrome but chrome flags missing; no mimeTypes</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
deal with some bugs
</commit_message>
<xml_diff>
--- a/data/level1_analysis.xlsx
+++ b/data/level1_analysis.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D129"/>
+  <dimension ref="A1:E205"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,10 +446,15 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>timestamp</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>is_bot</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>reasons</t>
         </is>
@@ -462,12 +467,17 @@
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
-      <c r="C2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2025-09-13T12:25:40</t>
+        </is>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -478,12 +488,17 @@
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
-      <c r="C3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2025-09-13T12:25:42</t>
+        </is>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -494,12 +509,17 @@
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
-      <c r="C4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>no plugins; UA contains Chrome but chrome flags missing; no mimeTypes</t>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2025-09-13T13:23:37</t>
+        </is>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>no plugins; no mimeTypes</t>
         </is>
       </c>
     </row>
@@ -510,12 +530,17 @@
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
-      <c r="C5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>no plugins; UA contains Chrome but chrome flags missing; no mimeTypes</t>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2025-09-13T13:24:09</t>
+        </is>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>no plugins; no mimeTypes</t>
         </is>
       </c>
     </row>
@@ -526,12 +551,17 @@
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
-      <c r="C6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>no plugins; UA contains Chrome but chrome flags missing; no mimeTypes</t>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2025-09-13T13:24:14</t>
+        </is>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>no plugins; no mimeTypes</t>
         </is>
       </c>
     </row>
@@ -542,12 +572,17 @@
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
-      <c r="C7" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>no plugins; UA contains Chrome but chrome flags missing; no mimeTypes</t>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2025-09-13T13:24:23</t>
+        </is>
+      </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>no plugins; no mimeTypes</t>
         </is>
       </c>
     </row>
@@ -558,12 +593,17 @@
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
-      <c r="C8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>no plugins; UA contains Chrome but chrome flags missing; no mimeTypes</t>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2025-09-13T13:24:25</t>
+        </is>
+      </c>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>no plugins; no mimeTypes</t>
         </is>
       </c>
     </row>
@@ -574,12 +614,17 @@
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
-      <c r="C9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2025-09-13T13:37:24</t>
+        </is>
+      </c>
+      <c r="D9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -590,12 +635,17 @@
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
-      <c r="C10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>no plugins; UA contains Chrome but chrome flags missing; no mimeTypes</t>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2025-09-13T13:40:59</t>
+        </is>
+      </c>
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>no plugins; no mimeTypes</t>
         </is>
       </c>
     </row>
@@ -606,12 +656,17 @@
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
-      <c r="C11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>no plugins; UA contains Chrome but chrome flags missing; no mimeTypes</t>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2025-09-13T13:42:38</t>
+        </is>
+      </c>
+      <c r="D11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>no plugins; no mimeTypes</t>
         </is>
       </c>
     </row>
@@ -622,12 +677,17 @@
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
-      <c r="C12" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>no plugins; UA contains Chrome but chrome flags missing; no mimeTypes</t>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2025-09-13T13:42:41</t>
+        </is>
+      </c>
+      <c r="D12" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>no plugins; no mimeTypes</t>
         </is>
       </c>
     </row>
@@ -638,12 +698,17 @@
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
-      <c r="C13" t="b">
-        <v>1</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>no plugins; UA contains Chrome but chrome flags missing; no mimeTypes; outerVsScreenWidth suspicious=690</t>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2025-09-13T13:43:43</t>
+        </is>
+      </c>
+      <c r="D13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>no plugins; no mimeTypes; outerVsScreenWidth suspicious=690</t>
         </is>
       </c>
     </row>
@@ -654,12 +719,17 @@
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
-      <c r="C14" t="b">
-        <v>1</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>no plugins; UA contains Chrome but chrome flags missing; no mimeTypes; outerVsScreenWidth suspicious=690</t>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2025-09-13T13:43:46</t>
+        </is>
+      </c>
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>no plugins; no mimeTypes; outerVsScreenWidth suspicious=690</t>
         </is>
       </c>
     </row>
@@ -670,12 +740,17 @@
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
-      <c r="C15" t="b">
-        <v>1</v>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2025-09-13T13:54:44</t>
+        </is>
+      </c>
+      <c r="D15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -686,12 +761,17 @@
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
-      <c r="C16" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>looks normal</t>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2025-09-13T13:54:52</t>
+        </is>
+      </c>
+      <c r="D16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>chrome.runtime unexpectedly present</t>
         </is>
       </c>
     </row>
@@ -702,12 +782,17 @@
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
-      <c r="C17" t="b">
-        <v>1</v>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>webdriver=true; no plugins; UA contains Chrome but chrome flags missing; no mimeTypes</t>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2025-09-15T11:58:03</t>
+        </is>
+      </c>
+      <c r="D17" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>webdriver=true; no plugins; no mimeTypes</t>
         </is>
       </c>
     </row>
@@ -718,12 +803,17 @@
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
-      <c r="C18" t="b">
-        <v>1</v>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>webdriver=true; no plugins; UA contains Chrome but chrome flags missing; no mimeTypes</t>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2025-09-15T11:58:18</t>
+        </is>
+      </c>
+      <c r="D18" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>webdriver=true; no plugins; no mimeTypes</t>
         </is>
       </c>
     </row>
@@ -734,12 +824,17 @@
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
-      <c r="C19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2025-09-15T13:03:46</t>
+        </is>
+      </c>
+      <c r="D19" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -750,12 +845,17 @@
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
-      <c r="C20" t="b">
-        <v>1</v>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>webdriver=true; no plugins; UA contains Chrome but chrome flags missing; no mimeTypes</t>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2025-09-15T14:03:26</t>
+        </is>
+      </c>
+      <c r="D20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>webdriver=true; no plugins; no mimeTypes</t>
         </is>
       </c>
     </row>
@@ -766,12 +866,17 @@
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
-      <c r="C21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2025-09-15T17:11:02</t>
+        </is>
+      </c>
+      <c r="D21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -782,12 +887,17 @@
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
-      <c r="C22" t="b">
-        <v>1</v>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2025-09-15T17:11:05</t>
+        </is>
+      </c>
+      <c r="D22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -798,10 +908,15 @@
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
-      <c r="C23" t="b">
-        <v>0</v>
-      </c>
-      <c r="D23" t="inlineStr">
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2025-09-15T17:11:45</t>
+        </is>
+      </c>
+      <c r="D23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E23" t="inlineStr">
         <is>
           <t>looks normal</t>
         </is>
@@ -814,10 +929,15 @@
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
-      <c r="C24" t="b">
-        <v>0</v>
-      </c>
-      <c r="D24" t="inlineStr">
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2025-09-15T17:11:47</t>
+        </is>
+      </c>
+      <c r="D24" t="b">
+        <v>0</v>
+      </c>
+      <c r="E24" t="inlineStr">
         <is>
           <t>looks normal</t>
         </is>
@@ -830,12 +950,17 @@
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
-      <c r="C25" t="b">
-        <v>1</v>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>webdriver=true; no plugins; no mimeTypes</t>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2025-09-16T13:25:10</t>
+        </is>
+      </c>
+      <c r="D25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>webdriver=true; no plugins; chrome.runtime unexpectedly present; no mimeTypes</t>
         </is>
       </c>
     </row>
@@ -846,12 +971,17 @@
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
-      <c r="C26" t="b">
-        <v>1</v>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing; outerVsScreenWidth suspicious=-270</t>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2025-09-16T15:41:16</t>
+        </is>
+      </c>
+      <c r="D26" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>outerVsScreenWidth suspicious=-270</t>
         </is>
       </c>
     </row>
@@ -862,12 +992,17 @@
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
-      <c r="C27" t="b">
-        <v>1</v>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing; outerVsScreenWidth suspicious=-270</t>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2025-09-16T15:41:22</t>
+        </is>
+      </c>
+      <c r="D27" t="b">
+        <v>1</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>outerVsScreenWidth suspicious=-270</t>
         </is>
       </c>
     </row>
@@ -878,12 +1013,17 @@
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
-      <c r="C28" t="b">
-        <v>1</v>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>2025-09-17T06:57:11</t>
+        </is>
+      </c>
+      <c r="D28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -894,12 +1034,17 @@
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
-      <c r="C29" t="b">
-        <v>1</v>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>2025-09-17T06:57:11</t>
+        </is>
+      </c>
+      <c r="D29" t="b">
+        <v>0</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -910,12 +1055,17 @@
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
-      <c r="C30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>looks normal</t>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>2025-09-17T06:57:14</t>
+        </is>
+      </c>
+      <c r="D30" t="b">
+        <v>1</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>chrome.runtime unexpectedly present</t>
         </is>
       </c>
     </row>
@@ -926,12 +1076,17 @@
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
-      <c r="C31" t="b">
-        <v>1</v>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>no plugins; UA contains Chrome but chrome flags missing; no mimeTypes</t>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>2025-09-17T07:04:37</t>
+        </is>
+      </c>
+      <c r="D31" t="b">
+        <v>1</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>no plugins; no mimeTypes</t>
         </is>
       </c>
     </row>
@@ -942,12 +1097,17 @@
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
-      <c r="C32" t="b">
-        <v>1</v>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>no plugins; UA contains Chrome but chrome flags missing; no mimeTypes</t>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>2025-09-17T07:04:39</t>
+        </is>
+      </c>
+      <c r="D32" t="b">
+        <v>1</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>no plugins; no mimeTypes</t>
         </is>
       </c>
     </row>
@@ -958,12 +1118,17 @@
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
-      <c r="C33" t="b">
-        <v>1</v>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>2025-09-18T08:13:30</t>
+        </is>
+      </c>
+      <c r="D33" t="b">
+        <v>0</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -974,12 +1139,17 @@
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
-      <c r="C34" t="b">
-        <v>1</v>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>2025-09-18T08:13:30</t>
+        </is>
+      </c>
+      <c r="D34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -990,12 +1160,17 @@
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
-      <c r="C35" t="b">
-        <v>1</v>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>2025-09-18T08:13:33</t>
+        </is>
+      </c>
+      <c r="D35" t="b">
+        <v>0</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1006,12 +1181,17 @@
         </is>
       </c>
       <c r="B36" t="inlineStr"/>
-      <c r="C36" t="b">
-        <v>1</v>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>2025-09-18T08:13:34</t>
+        </is>
+      </c>
+      <c r="D36" t="b">
+        <v>0</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1022,12 +1202,17 @@
         </is>
       </c>
       <c r="B37" t="inlineStr"/>
-      <c r="C37" t="b">
-        <v>1</v>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>2025-09-18T08:13:34</t>
+        </is>
+      </c>
+      <c r="D37" t="b">
+        <v>0</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1038,12 +1223,17 @@
         </is>
       </c>
       <c r="B38" t="inlineStr"/>
-      <c r="C38" t="b">
-        <v>1</v>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>2025-09-18T12:42:01</t>
+        </is>
+      </c>
+      <c r="D38" t="b">
+        <v>0</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1054,12 +1244,17 @@
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
-      <c r="C39" t="b">
-        <v>1</v>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>2025-09-18T12:42:04</t>
+        </is>
+      </c>
+      <c r="D39" t="b">
+        <v>0</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1070,12 +1265,17 @@
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
-      <c r="C40" t="b">
-        <v>1</v>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>2025-09-18T12:42:11</t>
+        </is>
+      </c>
+      <c r="D40" t="b">
+        <v>0</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1086,12 +1286,17 @@
         </is>
       </c>
       <c r="B41" t="inlineStr"/>
-      <c r="C41" t="b">
-        <v>1</v>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>2025-09-18T12:42:13</t>
+        </is>
+      </c>
+      <c r="D41" t="b">
+        <v>0</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1102,12 +1307,17 @@
         </is>
       </c>
       <c r="B42" t="inlineStr"/>
-      <c r="C42" t="b">
-        <v>1</v>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>2025-09-18T12:42:26</t>
+        </is>
+      </c>
+      <c r="D42" t="b">
+        <v>0</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1118,12 +1328,17 @@
         </is>
       </c>
       <c r="B43" t="inlineStr"/>
-      <c r="C43" t="b">
-        <v>1</v>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>2025-09-18T12:42:28</t>
+        </is>
+      </c>
+      <c r="D43" t="b">
+        <v>0</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1134,12 +1349,17 @@
         </is>
       </c>
       <c r="B44" t="inlineStr"/>
-      <c r="C44" t="b">
-        <v>1</v>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>2025-09-18T12:44:33</t>
+        </is>
+      </c>
+      <c r="D44" t="b">
+        <v>0</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1150,12 +1370,17 @@
         </is>
       </c>
       <c r="B45" t="inlineStr"/>
-      <c r="C45" t="b">
-        <v>1</v>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>2025-09-18T12:45:51</t>
+        </is>
+      </c>
+      <c r="D45" t="b">
+        <v>0</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1166,12 +1391,17 @@
         </is>
       </c>
       <c r="B46" t="inlineStr"/>
-      <c r="C46" t="b">
-        <v>1</v>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>2025-09-18T13:00:55</t>
+        </is>
+      </c>
+      <c r="D46" t="b">
+        <v>0</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1182,12 +1412,17 @@
         </is>
       </c>
       <c r="B47" t="inlineStr"/>
-      <c r="C47" t="b">
-        <v>1</v>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>2025-09-18T13:00:58</t>
+        </is>
+      </c>
+      <c r="D47" t="b">
+        <v>0</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1198,12 +1433,17 @@
         </is>
       </c>
       <c r="B48" t="inlineStr"/>
-      <c r="C48" t="b">
-        <v>1</v>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing; outerVsScreenWidth suspicious=-270</t>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>2025-09-18T13:31:55</t>
+        </is>
+      </c>
+      <c r="D48" t="b">
+        <v>1</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>outerVsScreenWidth suspicious=-270</t>
         </is>
       </c>
     </row>
@@ -1214,12 +1454,17 @@
         </is>
       </c>
       <c r="B49" t="inlineStr"/>
-      <c r="C49" t="b">
-        <v>1</v>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing; outerVsScreenWidth suspicious=-1470</t>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>2025-09-18T13:32:02</t>
+        </is>
+      </c>
+      <c r="D49" t="b">
+        <v>1</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>outerVsScreenWidth suspicious=-1470</t>
         </is>
       </c>
     </row>
@@ -1230,12 +1475,17 @@
         </is>
       </c>
       <c r="B50" t="inlineStr"/>
-      <c r="C50" t="b">
-        <v>1</v>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>2025-09-18T14:02:57</t>
+        </is>
+      </c>
+      <c r="D50" t="b">
+        <v>0</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1246,12 +1496,17 @@
         </is>
       </c>
       <c r="B51" t="inlineStr"/>
-      <c r="C51" t="b">
-        <v>1</v>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>2025-09-18T14:02:58</t>
+        </is>
+      </c>
+      <c r="D51" t="b">
+        <v>0</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1262,12 +1517,17 @@
         </is>
       </c>
       <c r="B52" t="inlineStr"/>
-      <c r="C52" t="b">
-        <v>1</v>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>2025-09-18T14:03:06</t>
+        </is>
+      </c>
+      <c r="D52" t="b">
+        <v>0</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1278,12 +1538,17 @@
         </is>
       </c>
       <c r="B53" t="inlineStr"/>
-      <c r="C53" t="b">
-        <v>1</v>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>2025-09-18T14:04:48</t>
+        </is>
+      </c>
+      <c r="D53" t="b">
+        <v>0</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1294,12 +1559,17 @@
         </is>
       </c>
       <c r="B54" t="inlineStr"/>
-      <c r="C54" t="b">
-        <v>1</v>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>2025-09-18T14:04:53</t>
+        </is>
+      </c>
+      <c r="D54" t="b">
+        <v>0</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1310,12 +1580,17 @@
         </is>
       </c>
       <c r="B55" t="inlineStr"/>
-      <c r="C55" t="b">
-        <v>1</v>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>2025-09-18T14:15:56</t>
+        </is>
+      </c>
+      <c r="D55" t="b">
+        <v>0</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1326,12 +1601,17 @@
         </is>
       </c>
       <c r="B56" t="inlineStr"/>
-      <c r="C56" t="b">
-        <v>1</v>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>2025-09-18T14:16:21</t>
+        </is>
+      </c>
+      <c r="D56" t="b">
+        <v>0</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1342,12 +1622,17 @@
         </is>
       </c>
       <c r="B57" t="inlineStr"/>
-      <c r="C57" t="b">
-        <v>1</v>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>2025-09-18T14:16:23</t>
+        </is>
+      </c>
+      <c r="D57" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1358,12 +1643,17 @@
         </is>
       </c>
       <c r="B58" t="inlineStr"/>
-      <c r="C58" t="b">
-        <v>1</v>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>2025-09-18T14:17:08</t>
+        </is>
+      </c>
+      <c r="D58" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1374,12 +1664,17 @@
         </is>
       </c>
       <c r="B59" t="inlineStr"/>
-      <c r="C59" t="b">
-        <v>1</v>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>2025-09-18T14:17:12</t>
+        </is>
+      </c>
+      <c r="D59" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1390,12 +1685,17 @@
         </is>
       </c>
       <c r="B60" t="inlineStr"/>
-      <c r="C60" t="b">
-        <v>1</v>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>2025-09-18T14:17:16</t>
+        </is>
+      </c>
+      <c r="D60" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1406,12 +1706,17 @@
         </is>
       </c>
       <c r="B61" t="inlineStr"/>
-      <c r="C61" t="b">
-        <v>1</v>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>2025-09-18T14:29:52</t>
+        </is>
+      </c>
+      <c r="D61" t="b">
+        <v>0</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1422,12 +1727,17 @@
         </is>
       </c>
       <c r="B62" t="inlineStr"/>
-      <c r="C62" t="b">
-        <v>1</v>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing; outerVsScreenWidth suspicious=-1707</t>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>2025-09-18T14:29:54</t>
+        </is>
+      </c>
+      <c r="D62" t="b">
+        <v>1</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>outerVsScreenWidth suspicious=-1707</t>
         </is>
       </c>
     </row>
@@ -1438,12 +1748,17 @@
         </is>
       </c>
       <c r="B63" t="inlineStr"/>
-      <c r="C63" t="b">
-        <v>1</v>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>2025-09-19T03:19:52</t>
+        </is>
+      </c>
+      <c r="D63" t="b">
+        <v>0</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1454,12 +1769,17 @@
         </is>
       </c>
       <c r="B64" t="inlineStr"/>
-      <c r="C64" t="b">
-        <v>1</v>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>2025-09-19T03:19:53</t>
+        </is>
+      </c>
+      <c r="D64" t="b">
+        <v>0</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1470,12 +1790,17 @@
         </is>
       </c>
       <c r="B65" t="inlineStr"/>
-      <c r="C65" t="b">
-        <v>1</v>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>2025-09-19T03:20:09</t>
+        </is>
+      </c>
+      <c r="D65" t="b">
+        <v>0</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1486,12 +1811,17 @@
         </is>
       </c>
       <c r="B66" t="inlineStr"/>
-      <c r="C66" t="b">
-        <v>1</v>
-      </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>2025-09-19T03:20:10</t>
+        </is>
+      </c>
+      <c r="D66" t="b">
+        <v>0</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1502,12 +1832,17 @@
         </is>
       </c>
       <c r="B67" t="inlineStr"/>
-      <c r="C67" t="b">
-        <v>1</v>
-      </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>2025-09-19T03:20:41</t>
+        </is>
+      </c>
+      <c r="D67" t="b">
+        <v>0</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1518,12 +1853,17 @@
         </is>
       </c>
       <c r="B68" t="inlineStr"/>
-      <c r="C68" t="b">
-        <v>1</v>
-      </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>2025-09-19T03:28:53</t>
+        </is>
+      </c>
+      <c r="D68" t="b">
+        <v>0</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1534,12 +1874,17 @@
         </is>
       </c>
       <c r="B69" t="inlineStr"/>
-      <c r="C69" t="b">
-        <v>1</v>
-      </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>2025-09-19T03:28:54</t>
+        </is>
+      </c>
+      <c r="D69" t="b">
+        <v>0</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1550,12 +1895,17 @@
         </is>
       </c>
       <c r="B70" t="inlineStr"/>
-      <c r="C70" t="b">
-        <v>1</v>
-      </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>2025-09-19T03:28:55</t>
+        </is>
+      </c>
+      <c r="D70" t="b">
+        <v>0</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1566,12 +1916,17 @@
         </is>
       </c>
       <c r="B71" t="inlineStr"/>
-      <c r="C71" t="b">
-        <v>1</v>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>2025-09-19T03:28:59</t>
+        </is>
+      </c>
+      <c r="D71" t="b">
+        <v>0</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1582,12 +1937,17 @@
         </is>
       </c>
       <c r="B72" t="inlineStr"/>
-      <c r="C72" t="b">
-        <v>1</v>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>2025-09-19T08:43:41</t>
+        </is>
+      </c>
+      <c r="D72" t="b">
+        <v>0</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1598,12 +1958,17 @@
         </is>
       </c>
       <c r="B73" t="inlineStr"/>
-      <c r="C73" t="b">
-        <v>1</v>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>2025-09-19T09:02:07</t>
+        </is>
+      </c>
+      <c r="D73" t="b">
+        <v>0</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1614,12 +1979,17 @@
         </is>
       </c>
       <c r="B74" t="inlineStr"/>
-      <c r="C74" t="b">
-        <v>1</v>
-      </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>2025-09-19T09:02:10</t>
+        </is>
+      </c>
+      <c r="D74" t="b">
+        <v>0</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1630,12 +2000,17 @@
         </is>
       </c>
       <c r="B75" t="inlineStr"/>
-      <c r="C75" t="b">
-        <v>1</v>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>2025-09-19T09:02:26</t>
+        </is>
+      </c>
+      <c r="D75" t="b">
+        <v>0</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1646,12 +2021,17 @@
         </is>
       </c>
       <c r="B76" t="inlineStr"/>
-      <c r="C76" t="b">
-        <v>1</v>
-      </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>2025-09-19T10:16:36</t>
+        </is>
+      </c>
+      <c r="D76" t="b">
+        <v>0</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1662,12 +2042,17 @@
         </is>
       </c>
       <c r="B77" t="inlineStr"/>
-      <c r="C77" t="b">
-        <v>1</v>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>2025-09-19T10:16:38</t>
+        </is>
+      </c>
+      <c r="D77" t="b">
+        <v>0</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1678,12 +2063,17 @@
         </is>
       </c>
       <c r="B78" t="inlineStr"/>
-      <c r="C78" t="b">
-        <v>1</v>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>2025-09-19T10:16:47</t>
+        </is>
+      </c>
+      <c r="D78" t="b">
+        <v>0</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1694,12 +2084,17 @@
         </is>
       </c>
       <c r="B79" t="inlineStr"/>
-      <c r="C79" t="b">
-        <v>1</v>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>2025-09-19T14:46:37</t>
+        </is>
+      </c>
+      <c r="D79" t="b">
+        <v>0</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1710,12 +2105,17 @@
         </is>
       </c>
       <c r="B80" t="inlineStr"/>
-      <c r="C80" t="b">
-        <v>1</v>
-      </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>outerVsScreenWidth suspicious=-270</t>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>2025-09-19T14:51:37</t>
+        </is>
+      </c>
+      <c r="D80" t="b">
+        <v>1</v>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>chrome.runtime unexpectedly present; outerVsScreenWidth suspicious=-270</t>
         </is>
       </c>
     </row>
@@ -1726,12 +2126,17 @@
         </is>
       </c>
       <c r="B81" t="inlineStr"/>
-      <c r="C81" t="b">
-        <v>1</v>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>outerVsScreenWidth suspicious=-270</t>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>2025-09-19T14:51:39</t>
+        </is>
+      </c>
+      <c r="D81" t="b">
+        <v>1</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>chrome.runtime unexpectedly present; outerVsScreenWidth suspicious=-270</t>
         </is>
       </c>
     </row>
@@ -1742,12 +2147,17 @@
         </is>
       </c>
       <c r="B82" t="inlineStr"/>
-      <c r="C82" t="b">
-        <v>1</v>
-      </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>outerVsScreenWidth suspicious=-270</t>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>2025-09-19T14:59:14</t>
+        </is>
+      </c>
+      <c r="D82" t="b">
+        <v>1</v>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>chrome.runtime unexpectedly present; outerVsScreenWidth suspicious=-270</t>
         </is>
       </c>
     </row>
@@ -1758,12 +2168,17 @@
         </is>
       </c>
       <c r="B83" t="inlineStr"/>
-      <c r="C83" t="b">
-        <v>1</v>
-      </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>outerVsScreenWidth suspicious=-270</t>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>2025-09-19T14:59:17</t>
+        </is>
+      </c>
+      <c r="D83" t="b">
+        <v>1</v>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>chrome.runtime unexpectedly present; outerVsScreenWidth suspicious=-270</t>
         </is>
       </c>
     </row>
@@ -1774,12 +2189,17 @@
         </is>
       </c>
       <c r="B84" t="inlineStr"/>
-      <c r="C84" t="b">
-        <v>1</v>
-      </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>2025-09-19T15:36:20</t>
+        </is>
+      </c>
+      <c r="D84" t="b">
+        <v>0</v>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1790,12 +2210,17 @@
         </is>
       </c>
       <c r="B85" t="inlineStr"/>
-      <c r="C85" t="b">
-        <v>1</v>
-      </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>2025-09-19T15:36:22</t>
+        </is>
+      </c>
+      <c r="D85" t="b">
+        <v>0</v>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1806,12 +2231,17 @@
         </is>
       </c>
       <c r="B86" t="inlineStr"/>
-      <c r="C86" t="b">
-        <v>1</v>
-      </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>2025-09-19T15:36:33</t>
+        </is>
+      </c>
+      <c r="D86" t="b">
+        <v>0</v>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1822,12 +2252,17 @@
         </is>
       </c>
       <c r="B87" t="inlineStr"/>
-      <c r="C87" t="b">
-        <v>1</v>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>2025-09-19T15:37:20</t>
+        </is>
+      </c>
+      <c r="D87" t="b">
+        <v>0</v>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1838,12 +2273,17 @@
         </is>
       </c>
       <c r="B88" t="inlineStr"/>
-      <c r="C88" t="b">
-        <v>1</v>
-      </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>2025-09-19T15:52:14</t>
+        </is>
+      </c>
+      <c r="D88" t="b">
+        <v>0</v>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1854,12 +2294,17 @@
         </is>
       </c>
       <c r="B89" t="inlineStr"/>
-      <c r="C89" t="b">
-        <v>1</v>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing; outerVsScreenWidth suspicious=-1707</t>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>2025-09-19T15:52:16</t>
+        </is>
+      </c>
+      <c r="D89" t="b">
+        <v>1</v>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>outerVsScreenWidth suspicious=-1707</t>
         </is>
       </c>
     </row>
@@ -1870,12 +2315,17 @@
         </is>
       </c>
       <c r="B90" t="inlineStr"/>
-      <c r="C90" t="b">
-        <v>1</v>
-      </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>2025-09-19T16:16:53</t>
+        </is>
+      </c>
+      <c r="D90" t="b">
+        <v>0</v>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1886,12 +2336,17 @@
         </is>
       </c>
       <c r="B91" t="inlineStr"/>
-      <c r="C91" t="b">
-        <v>1</v>
-      </c>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>2025-09-19T16:17:17</t>
+        </is>
+      </c>
+      <c r="D91" t="b">
+        <v>0</v>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1902,12 +2357,17 @@
         </is>
       </c>
       <c r="B92" t="inlineStr"/>
-      <c r="C92" t="b">
-        <v>1</v>
-      </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>2025-09-19T16:17:49</t>
+        </is>
+      </c>
+      <c r="D92" t="b">
+        <v>0</v>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1918,12 +2378,17 @@
         </is>
       </c>
       <c r="B93" t="inlineStr"/>
-      <c r="C93" t="b">
-        <v>1</v>
-      </c>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>2025-09-19T16:33:13</t>
+        </is>
+      </c>
+      <c r="D93" t="b">
+        <v>0</v>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1934,12 +2399,17 @@
         </is>
       </c>
       <c r="B94" t="inlineStr"/>
-      <c r="C94" t="b">
-        <v>1</v>
-      </c>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing; outerVsScreenWidth suspicious=-1707</t>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>2025-09-19T16:33:15</t>
+        </is>
+      </c>
+      <c r="D94" t="b">
+        <v>1</v>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>outerVsScreenWidth suspicious=-1707</t>
         </is>
       </c>
     </row>
@@ -1950,12 +2420,17 @@
         </is>
       </c>
       <c r="B95" t="inlineStr"/>
-      <c r="C95" t="b">
-        <v>1</v>
-      </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>2025-09-20T13:50:04</t>
+        </is>
+      </c>
+      <c r="D95" t="b">
+        <v>0</v>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -1966,10 +2441,15 @@
         </is>
       </c>
       <c r="B96" t="inlineStr"/>
-      <c r="C96" t="b">
-        <v>0</v>
-      </c>
-      <c r="D96" t="inlineStr">
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>2025-09-23T05:57:47</t>
+        </is>
+      </c>
+      <c r="D96" t="b">
+        <v>0</v>
+      </c>
+      <c r="E96" t="inlineStr">
         <is>
           <t>looks normal</t>
         </is>
@@ -1982,10 +2462,15 @@
         </is>
       </c>
       <c r="B97" t="inlineStr"/>
-      <c r="C97" t="b">
-        <v>0</v>
-      </c>
-      <c r="D97" t="inlineStr">
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>2025-09-23T05:57:50</t>
+        </is>
+      </c>
+      <c r="D97" t="b">
+        <v>0</v>
+      </c>
+      <c r="E97" t="inlineStr">
         <is>
           <t>looks normal</t>
         </is>
@@ -1998,12 +2483,17 @@
         </is>
       </c>
       <c r="B98" t="inlineStr"/>
-      <c r="C98" t="b">
-        <v>1</v>
-      </c>
-      <c r="D98" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>2025-09-23T08:14:45</t>
+        </is>
+      </c>
+      <c r="D98" t="b">
+        <v>0</v>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -2014,12 +2504,17 @@
         </is>
       </c>
       <c r="B99" t="inlineStr"/>
-      <c r="C99" t="b">
-        <v>1</v>
-      </c>
-      <c r="D99" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>2025-09-23T08:15:41</t>
+        </is>
+      </c>
+      <c r="D99" t="b">
+        <v>0</v>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -2030,12 +2525,17 @@
         </is>
       </c>
       <c r="B100" t="inlineStr"/>
-      <c r="C100" t="b">
-        <v>1</v>
-      </c>
-      <c r="D100" t="inlineStr">
-        <is>
-          <t>webdriver=true; no plugins; UA contains Chrome but chrome flags missing; no mimeTypes; outerVsScreenWidth suspicious=224</t>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>2025-09-23T09:11:48</t>
+        </is>
+      </c>
+      <c r="D100" t="b">
+        <v>1</v>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>webdriver=true; no plugins; no mimeTypes; outerVsScreenWidth suspicious=224</t>
         </is>
       </c>
     </row>
@@ -2046,12 +2546,17 @@
         </is>
       </c>
       <c r="B101" t="inlineStr"/>
-      <c r="C101" t="b">
-        <v>1</v>
-      </c>
-      <c r="D101" t="inlineStr">
-        <is>
-          <t>webdriver=true; no plugins; UA contains Chrome but chrome flags missing; no mimeTypes; outerVsScreenWidth suspicious=224</t>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>2025-09-23T09:12:28</t>
+        </is>
+      </c>
+      <c r="D101" t="b">
+        <v>1</v>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>webdriver=true; no plugins; no mimeTypes; outerVsScreenWidth suspicious=224</t>
         </is>
       </c>
     </row>
@@ -2062,12 +2567,17 @@
         </is>
       </c>
       <c r="B102" t="inlineStr"/>
-      <c r="C102" t="b">
-        <v>1</v>
-      </c>
-      <c r="D102" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>2025-09-23T09:14:43</t>
+        </is>
+      </c>
+      <c r="D102" t="b">
+        <v>0</v>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -2078,12 +2588,17 @@
         </is>
       </c>
       <c r="B103" t="inlineStr"/>
-      <c r="C103" t="b">
-        <v>1</v>
-      </c>
-      <c r="D103" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>2025-09-23T09:14:44</t>
+        </is>
+      </c>
+      <c r="D103" t="b">
+        <v>0</v>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -2094,12 +2609,17 @@
         </is>
       </c>
       <c r="B104" t="inlineStr"/>
-      <c r="C104" t="b">
-        <v>1</v>
-      </c>
-      <c r="D104" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>2025-09-23T09:14:44</t>
+        </is>
+      </c>
+      <c r="D104" t="b">
+        <v>0</v>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -2110,12 +2630,17 @@
         </is>
       </c>
       <c r="B105" t="inlineStr"/>
-      <c r="C105" t="b">
-        <v>1</v>
-      </c>
-      <c r="D105" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>2025-09-23T09:14:45</t>
+        </is>
+      </c>
+      <c r="D105" t="b">
+        <v>0</v>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -2126,12 +2651,17 @@
         </is>
       </c>
       <c r="B106" t="inlineStr"/>
-      <c r="C106" t="b">
-        <v>1</v>
-      </c>
-      <c r="D106" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>2025-09-23T09:14:46</t>
+        </is>
+      </c>
+      <c r="D106" t="b">
+        <v>0</v>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -2142,12 +2672,17 @@
         </is>
       </c>
       <c r="B107" t="inlineStr"/>
-      <c r="C107" t="b">
-        <v>1</v>
-      </c>
-      <c r="D107" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>2025-09-23T09:14:48</t>
+        </is>
+      </c>
+      <c r="D107" t="b">
+        <v>0</v>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -2158,12 +2693,17 @@
         </is>
       </c>
       <c r="B108" t="inlineStr"/>
-      <c r="C108" t="b">
-        <v>1</v>
-      </c>
-      <c r="D108" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>2025-09-23T09:14:57</t>
+        </is>
+      </c>
+      <c r="D108" t="b">
+        <v>0</v>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -2174,12 +2714,17 @@
         </is>
       </c>
       <c r="B109" t="inlineStr"/>
-      <c r="C109" t="b">
-        <v>1</v>
-      </c>
-      <c r="D109" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>2025-09-23T09:28:40</t>
+        </is>
+      </c>
+      <c r="D109" t="b">
+        <v>0</v>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -2190,12 +2735,17 @@
         </is>
       </c>
       <c r="B110" t="inlineStr"/>
-      <c r="C110" t="b">
-        <v>1</v>
-      </c>
-      <c r="D110" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>2025-09-23T09:28:44</t>
+        </is>
+      </c>
+      <c r="D110" t="b">
+        <v>0</v>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -2206,12 +2756,17 @@
         </is>
       </c>
       <c r="B111" t="inlineStr"/>
-      <c r="C111" t="b">
-        <v>1</v>
-      </c>
-      <c r="D111" t="inlineStr">
-        <is>
-          <t>webdriver=true; no plugins; UA contains Chrome but chrome flags missing; no mimeTypes; outerVsScreenWidth suspicious=224</t>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>2025-09-23T10:51:46</t>
+        </is>
+      </c>
+      <c r="D111" t="b">
+        <v>1</v>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>webdriver=true; no plugins; no mimeTypes; outerVsScreenWidth suspicious=224</t>
         </is>
       </c>
     </row>
@@ -2222,12 +2777,17 @@
         </is>
       </c>
       <c r="B112" t="inlineStr"/>
-      <c r="C112" t="b">
-        <v>1</v>
-      </c>
-      <c r="D112" t="inlineStr">
-        <is>
-          <t>webdriver=true; no plugins; UA contains Chrome but chrome flags missing; no mimeTypes; outerVsScreenWidth suspicious=224</t>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>2025-09-23T10:51:47</t>
+        </is>
+      </c>
+      <c r="D112" t="b">
+        <v>1</v>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>webdriver=true; no plugins; no mimeTypes; outerVsScreenWidth suspicious=224</t>
         </is>
       </c>
     </row>
@@ -2238,12 +2798,17 @@
         </is>
       </c>
       <c r="B113" t="inlineStr"/>
-      <c r="C113" t="b">
-        <v>1</v>
-      </c>
-      <c r="D113" t="inlineStr">
-        <is>
-          <t>webdriver=true; no plugins; UA contains Chrome but chrome flags missing; no mimeTypes; outerVsScreenWidth suspicious=224</t>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>2025-09-23T10:51:51</t>
+        </is>
+      </c>
+      <c r="D113" t="b">
+        <v>1</v>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>webdriver=true; no plugins; no mimeTypes; outerVsScreenWidth suspicious=224</t>
         </is>
       </c>
     </row>
@@ -2254,12 +2819,17 @@
         </is>
       </c>
       <c r="B114" t="inlineStr"/>
-      <c r="C114" t="b">
-        <v>1</v>
-      </c>
-      <c r="D114" t="inlineStr">
-        <is>
-          <t>UA contains Chrome but chrome flags missing</t>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>2025-09-25T08:48:20</t>
+        </is>
+      </c>
+      <c r="D114" t="b">
+        <v>0</v>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>
@@ -2270,10 +2840,15 @@
         </is>
       </c>
       <c r="B115" t="inlineStr"/>
-      <c r="C115" t="b">
-        <v>0</v>
-      </c>
-      <c r="D115" t="inlineStr">
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>2025-09-25T09:06:31</t>
+        </is>
+      </c>
+      <c r="D115" t="b">
+        <v>0</v>
+      </c>
+      <c r="E115" t="inlineStr">
         <is>
           <t>looks normal</t>
         </is>
@@ -2286,12 +2861,17 @@
         </is>
       </c>
       <c r="B116" t="inlineStr"/>
-      <c r="C116" t="b">
-        <v>1</v>
-      </c>
-      <c r="D116" t="inlineStr">
-        <is>
-          <t>webdriver=true; UA contains Chrome but chrome flags missing</t>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>2025-09-25T11:34:28</t>
+        </is>
+      </c>
+      <c r="D116" t="b">
+        <v>1</v>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>webdriver=true</t>
         </is>
       </c>
     </row>
@@ -2302,12 +2882,17 @@
         </is>
       </c>
       <c r="B117" t="inlineStr"/>
-      <c r="C117" t="b">
-        <v>1</v>
-      </c>
-      <c r="D117" t="inlineStr">
-        <is>
-          <t>webdriver=true; UA contains Chrome but chrome flags missing</t>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>2025-09-25T11:34:31</t>
+        </is>
+      </c>
+      <c r="D117" t="b">
+        <v>1</v>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>webdriver=true</t>
         </is>
       </c>
     </row>
@@ -2318,12 +2903,17 @@
         </is>
       </c>
       <c r="B118" t="inlineStr"/>
-      <c r="C118" t="b">
-        <v>1</v>
-      </c>
-      <c r="D118" t="inlineStr">
-        <is>
-          <t>webdriver=true; UA contains Chrome but chrome flags missing</t>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>2025-09-25T11:34:34</t>
+        </is>
+      </c>
+      <c r="D118" t="b">
+        <v>1</v>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>webdriver=true</t>
         </is>
       </c>
     </row>
@@ -2334,12 +2924,17 @@
         </is>
       </c>
       <c r="B119" t="inlineStr"/>
-      <c r="C119" t="b">
-        <v>1</v>
-      </c>
-      <c r="D119" t="inlineStr">
-        <is>
-          <t>webdriver=true; UA contains Chrome but chrome flags missing</t>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>2025-09-25T11:48:20</t>
+        </is>
+      </c>
+      <c r="D119" t="b">
+        <v>1</v>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>webdriver=true</t>
         </is>
       </c>
     </row>
@@ -2350,12 +2945,17 @@
         </is>
       </c>
       <c r="B120" t="inlineStr"/>
-      <c r="C120" t="b">
-        <v>1</v>
-      </c>
-      <c r="D120" t="inlineStr">
-        <is>
-          <t>webdriver=true; UA contains Chrome but chrome flags missing</t>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>2025-09-25T11:48:20</t>
+        </is>
+      </c>
+      <c r="D120" t="b">
+        <v>1</v>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>webdriver=true</t>
         </is>
       </c>
     </row>
@@ -2366,12 +2966,17 @@
         </is>
       </c>
       <c r="B121" t="inlineStr"/>
-      <c r="C121" t="b">
-        <v>1</v>
-      </c>
-      <c r="D121" t="inlineStr">
-        <is>
-          <t>webdriver=true; UA contains Chrome but chrome flags missing</t>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>2025-09-25T11:48:24</t>
+        </is>
+      </c>
+      <c r="D121" t="b">
+        <v>1</v>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>webdriver=true</t>
         </is>
       </c>
     </row>
@@ -2382,12 +2987,17 @@
         </is>
       </c>
       <c r="B122" t="inlineStr"/>
-      <c r="C122" t="b">
-        <v>1</v>
-      </c>
-      <c r="D122" t="inlineStr">
-        <is>
-          <t>webdriver=true; UA contains Chrome but chrome flags missing</t>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>2025-09-25T12:10:02</t>
+        </is>
+      </c>
+      <c r="D122" t="b">
+        <v>1</v>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>webdriver=true</t>
         </is>
       </c>
     </row>
@@ -2398,12 +3008,17 @@
         </is>
       </c>
       <c r="B123" t="inlineStr"/>
-      <c r="C123" t="b">
-        <v>1</v>
-      </c>
-      <c r="D123" t="inlineStr">
-        <is>
-          <t>webdriver=true; UA contains Chrome but chrome flags missing</t>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>2025-09-25T12:10:06</t>
+        </is>
+      </c>
+      <c r="D123" t="b">
+        <v>1</v>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>webdriver=true</t>
         </is>
       </c>
     </row>
@@ -2414,12 +3029,17 @@
         </is>
       </c>
       <c r="B124" t="inlineStr"/>
-      <c r="C124" t="b">
-        <v>1</v>
-      </c>
-      <c r="D124" t="inlineStr">
-        <is>
-          <t>no plugins; UA contains Chrome but chrome flags missing; no mimeTypes</t>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>2025-09-25T12:40:12</t>
+        </is>
+      </c>
+      <c r="D124" t="b">
+        <v>1</v>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>no plugins; no mimeTypes</t>
         </is>
       </c>
     </row>
@@ -2430,12 +3050,17 @@
         </is>
       </c>
       <c r="B125" t="inlineStr"/>
-      <c r="C125" t="b">
-        <v>1</v>
-      </c>
-      <c r="D125" t="inlineStr">
-        <is>
-          <t>no plugins; UA contains Chrome but chrome flags missing; no mimeTypes</t>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>2025-09-25T12:40:15</t>
+        </is>
+      </c>
+      <c r="D125" t="b">
+        <v>1</v>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>no plugins; no mimeTypes</t>
         </is>
       </c>
     </row>
@@ -2446,12 +3071,17 @@
         </is>
       </c>
       <c r="B126" t="inlineStr"/>
-      <c r="C126" t="b">
-        <v>1</v>
-      </c>
-      <c r="D126" t="inlineStr">
-        <is>
-          <t>no plugins; UA contains Chrome but chrome flags missing; no mimeTypes</t>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>2025-09-25T12:40:18</t>
+        </is>
+      </c>
+      <c r="D126" t="b">
+        <v>1</v>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>no plugins; no mimeTypes</t>
         </is>
       </c>
     </row>
@@ -2462,12 +3092,17 @@
         </is>
       </c>
       <c r="B127" t="inlineStr"/>
-      <c r="C127" t="b">
-        <v>1</v>
-      </c>
-      <c r="D127" t="inlineStr">
-        <is>
-          <t>no plugins; UA contains Chrome but chrome flags missing; no mimeTypes</t>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>2025-09-25T12:40:27</t>
+        </is>
+      </c>
+      <c r="D127" t="b">
+        <v>1</v>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>no plugins; no mimeTypes</t>
         </is>
       </c>
     </row>
@@ -2478,12 +3113,17 @@
         </is>
       </c>
       <c r="B128" t="inlineStr"/>
-      <c r="C128" t="b">
-        <v>1</v>
-      </c>
-      <c r="D128" t="inlineStr">
-        <is>
-          <t>no plugins; UA contains Chrome but chrome flags missing; no mimeTypes</t>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>2025-09-25T12:40:31</t>
+        </is>
+      </c>
+      <c r="D128" t="b">
+        <v>1</v>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>no plugins; no mimeTypes</t>
         </is>
       </c>
     </row>
@@ -2494,12 +3134,1613 @@
         </is>
       </c>
       <c r="B129" t="inlineStr"/>
-      <c r="C129" t="b">
-        <v>1</v>
-      </c>
-      <c r="D129" t="inlineStr">
-        <is>
-          <t>no plugins; UA contains Chrome but chrome flags missing; no mimeTypes</t>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>2025-09-25T12:40:36</t>
+        </is>
+      </c>
+      <c r="D129" t="b">
+        <v>1</v>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>no plugins; no mimeTypes</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>m.ik.k.am.u.e.rtio@gmail.com</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr"/>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>2025-09-25T14:13:02</t>
+        </is>
+      </c>
+      <c r="D130" t="b">
+        <v>0</v>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>m.ik.k.am.u.e.rtio@gmail.com</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr"/>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>2025-09-25T14:13:28</t>
+        </is>
+      </c>
+      <c r="D131" t="b">
+        <v>0</v>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr"/>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>2025-09-25T14:13:31</t>
+        </is>
+      </c>
+      <c r="D132" t="b">
+        <v>0</v>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>m.ik.k.am.u.e.rtio@gmail.com</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr"/>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>2025-09-25T14:14:24</t>
+        </is>
+      </c>
+      <c r="D133" t="b">
+        <v>0</v>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr"/>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>2025-09-25T14:14:27</t>
+        </is>
+      </c>
+      <c r="D134" t="b">
+        <v>0</v>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>m.ik.k.am.u.e.rtio@gmail.com</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr"/>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>2025-09-25T14:14:46</t>
+        </is>
+      </c>
+      <c r="D135" t="b">
+        <v>0</v>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr"/>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>2025-09-25T14:14:48</t>
+        </is>
+      </c>
+      <c r="D136" t="b">
+        <v>0</v>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr"/>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>2025-09-25T15:24:58</t>
+        </is>
+      </c>
+      <c r="D137" t="b">
+        <v>0</v>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr"/>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>2025-09-25T15:24:58</t>
+        </is>
+      </c>
+      <c r="D138" t="b">
+        <v>0</v>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr"/>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>2025-09-25T15:25:01</t>
+        </is>
+      </c>
+      <c r="D139" t="b">
+        <v>0</v>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr"/>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>2025-09-27T10:54:12</t>
+        </is>
+      </c>
+      <c r="D140" t="b">
+        <v>0</v>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr"/>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>2025-09-27T10:58:04</t>
+        </is>
+      </c>
+      <c r="D141" t="b">
+        <v>0</v>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr"/>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>2025-09-27T10:58:08</t>
+        </is>
+      </c>
+      <c r="D142" t="b">
+        <v>0</v>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr"/>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>2025-09-27T10:58:27</t>
+        </is>
+      </c>
+      <c r="D143" t="b">
+        <v>0</v>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr"/>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>2025-09-28T12:30:38</t>
+        </is>
+      </c>
+      <c r="D144" t="b">
+        <v>0</v>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr"/>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>2025-09-28T12:34:53</t>
+        </is>
+      </c>
+      <c r="D145" t="b">
+        <v>0</v>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr"/>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>2025-09-28T12:35:09</t>
+        </is>
+      </c>
+      <c r="D146" t="b">
+        <v>0</v>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr"/>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>2025-09-28T12:41:07</t>
+        </is>
+      </c>
+      <c r="D147" t="b">
+        <v>0</v>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr"/>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>2025-09-28T12:41:16</t>
+        </is>
+      </c>
+      <c r="D148" t="b">
+        <v>0</v>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr"/>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>2025-09-28T12:41:46</t>
+        </is>
+      </c>
+      <c r="D149" t="b">
+        <v>0</v>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr"/>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>2025-09-28T12:43:02</t>
+        </is>
+      </c>
+      <c r="D150" t="b">
+        <v>0</v>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr"/>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>2025-09-28T12:43:33</t>
+        </is>
+      </c>
+      <c r="D151" t="b">
+        <v>0</v>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr"/>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>2025-09-28T12:44:03</t>
+        </is>
+      </c>
+      <c r="D152" t="b">
+        <v>0</v>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr"/>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>2025-09-28T12:44:52</t>
+        </is>
+      </c>
+      <c r="D153" t="b">
+        <v>0</v>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr"/>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>2025-09-28T13:18:04</t>
+        </is>
+      </c>
+      <c r="D154" t="b">
+        <v>0</v>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr"/>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>2025-09-29T08:50:35</t>
+        </is>
+      </c>
+      <c r="D155" t="b">
+        <v>0</v>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr"/>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>2025-09-29T08:56:54</t>
+        </is>
+      </c>
+      <c r="D156" t="b">
+        <v>0</v>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr"/>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>2025-09-29T13:39:59</t>
+        </is>
+      </c>
+      <c r="D157" t="b">
+        <v>0</v>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr"/>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>2025-09-29T13:47:52</t>
+        </is>
+      </c>
+      <c r="D158" t="b">
+        <v>0</v>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr"/>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>2025-09-29T13:51:24</t>
+        </is>
+      </c>
+      <c r="D159" t="b">
+        <v>0</v>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr"/>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>2025-09-29T13:57:12</t>
+        </is>
+      </c>
+      <c r="D160" t="b">
+        <v>0</v>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>bot10</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr"/>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>2025-10-07T06:29:55</t>
+        </is>
+      </c>
+      <c r="D161" t="b">
+        <v>1</v>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>outerVsScreenWidth suspicious=-718</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr"/>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>2025-10-07T11:34:55</t>
+        </is>
+      </c>
+      <c r="D162" t="b">
+        <v>1</v>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>webdriver=true; no plugins; chrome.runtime unexpectedly present; no mimeTypes</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>bot10</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr"/>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>2025-10-08T12:19:51</t>
+        </is>
+      </c>
+      <c r="D163" t="b">
+        <v>1</v>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>outerVsScreenWidth suspicious=-1253</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>bot10</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr"/>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>2025-10-08T12:26:51</t>
+        </is>
+      </c>
+      <c r="D164" t="b">
+        <v>0</v>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr"/>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>2025-10-08T12:26:54</t>
+        </is>
+      </c>
+      <c r="D165" t="b">
+        <v>0</v>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr"/>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>2025-10-08T19:24:50</t>
+        </is>
+      </c>
+      <c r="D166" t="b">
+        <v>0</v>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr"/>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>2025-10-09T03:26:43</t>
+        </is>
+      </c>
+      <c r="D167" t="b">
+        <v>0</v>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr"/>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>2025-10-09T04:05:40</t>
+        </is>
+      </c>
+      <c r="D168" t="b">
+        <v>1</v>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>webdriver=true; no plugins; chrome.runtime unexpectedly present; no mimeTypes</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr"/>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>2025-10-09T04:06:20</t>
+        </is>
+      </c>
+      <c r="D169" t="b">
+        <v>0</v>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr"/>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>2025-10-09T04:06:23</t>
+        </is>
+      </c>
+      <c r="D170" t="b">
+        <v>0</v>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>bot11</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr"/>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>2025-10-09T07:12:25</t>
+        </is>
+      </c>
+      <c r="D171" t="b">
+        <v>1</v>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>webdriver=true</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr"/>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>2025-10-09T07:12:36</t>
+        </is>
+      </c>
+      <c r="D172" t="b">
+        <v>1</v>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>webdriver=true</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr"/>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>2025-10-09T17:01:04</t>
+        </is>
+      </c>
+      <c r="D173" t="b">
+        <v>0</v>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr"/>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>2025-10-09T17:16:46</t>
+        </is>
+      </c>
+      <c r="D174" t="b">
+        <v>0</v>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr"/>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>2025-10-09T17:17:14</t>
+        </is>
+      </c>
+      <c r="D175" t="b">
+        <v>0</v>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr"/>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>2025-10-09T17:17:17</t>
+        </is>
+      </c>
+      <c r="D176" t="b">
+        <v>0</v>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr"/>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>2025-10-09T17:22:35</t>
+        </is>
+      </c>
+      <c r="D177" t="b">
+        <v>0</v>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr"/>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>2025-10-09T17:22:38</t>
+        </is>
+      </c>
+      <c r="D178" t="b">
+        <v>0</v>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr"/>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>2025-10-09T17:23:15</t>
+        </is>
+      </c>
+      <c r="D179" t="b">
+        <v>0</v>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr"/>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>2025-10-09T17:23:17</t>
+        </is>
+      </c>
+      <c r="D180" t="b">
+        <v>0</v>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr"/>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>2025-10-09T17:23:30</t>
+        </is>
+      </c>
+      <c r="D181" t="b">
+        <v>0</v>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr"/>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>2025-10-09T17:23:34</t>
+        </is>
+      </c>
+      <c r="D182" t="b">
+        <v>0</v>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr"/>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>2025-10-09T17:23:37</t>
+        </is>
+      </c>
+      <c r="D183" t="b">
+        <v>0</v>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr"/>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>2025-10-09T17:26:37</t>
+        </is>
+      </c>
+      <c r="D184" t="b">
+        <v>0</v>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr"/>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>2025-10-09T17:29:19</t>
+        </is>
+      </c>
+      <c r="D185" t="b">
+        <v>0</v>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr"/>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>2025-10-09T17:29:22</t>
+        </is>
+      </c>
+      <c r="D186" t="b">
+        <v>0</v>
+      </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>bot03</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr"/>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>2025-10-10T14:27:20</t>
+        </is>
+      </c>
+      <c r="D187" t="b">
+        <v>1</v>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>chrome.runtime unexpectedly present</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr"/>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>2025-10-10T14:27:27</t>
+        </is>
+      </c>
+      <c r="D188" t="b">
+        <v>1</v>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>chrome.runtime unexpectedly present</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>bot02</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr"/>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>2025-10-12T11:06:15</t>
+        </is>
+      </c>
+      <c r="D189" t="b">
+        <v>0</v>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>bot02</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr"/>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>2025-10-12T15:59:54</t>
+        </is>
+      </c>
+      <c r="D190" t="b">
+        <v>0</v>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>bot02</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr"/>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>2025-10-12T16:14:57</t>
+        </is>
+      </c>
+      <c r="D191" t="b">
+        <v>0</v>
+      </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr"/>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>2025-10-12T16:15:01</t>
+        </is>
+      </c>
+      <c r="D192" t="b">
+        <v>0</v>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>bot13</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr"/>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>2025-10-13T05:53:01</t>
+        </is>
+      </c>
+      <c r="D193" t="b">
+        <v>1</v>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>webdriver=true</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr"/>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>2025-10-13T05:53:07</t>
+        </is>
+      </c>
+      <c r="D194" t="b">
+        <v>1</v>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>webdriver=true</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>bottest01</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr"/>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>2025-10-20T08:05:18</t>
+        </is>
+      </c>
+      <c r="D195" t="b">
+        <v>0</v>
+      </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr"/>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>2025-10-20T08:05:25</t>
+        </is>
+      </c>
+      <c r="D196" t="b">
+        <v>0</v>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>bottest01</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr"/>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>2025-10-20T08:38:05</t>
+        </is>
+      </c>
+      <c r="D197" t="b">
+        <v>0</v>
+      </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr"/>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>2025-10-20T08:38:10</t>
+        </is>
+      </c>
+      <c r="D198" t="b">
+        <v>0</v>
+      </c>
+      <c r="E198" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>bot15</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr"/>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>2025-10-20T10:53:22</t>
+        </is>
+      </c>
+      <c r="D199" t="b">
+        <v>0</v>
+      </c>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr"/>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>2025-10-20T10:53:28</t>
+        </is>
+      </c>
+      <c r="D200" t="b">
+        <v>0</v>
+      </c>
+      <c r="E200" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr"/>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>2025-10-20T10:53:34</t>
+        </is>
+      </c>
+      <c r="D201" t="b">
+        <v>0</v>
+      </c>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr"/>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>2025-10-25T16:45:03</t>
+        </is>
+      </c>
+      <c r="D202" t="b">
+        <v>0</v>
+      </c>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr"/>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>2025-10-28T01:34:05</t>
+        </is>
+      </c>
+      <c r="D203" t="b">
+        <v>0</v>
+      </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr"/>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>2025-10-28T01:40:10</t>
+        </is>
+      </c>
+      <c r="D204" t="b">
+        <v>0</v>
+      </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>looks normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>guest</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr"/>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>2025-10-28T01:40:29</t>
+        </is>
+      </c>
+      <c r="D205" t="b">
+        <v>0</v>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>looks normal</t>
         </is>
       </c>
     </row>

</xml_diff>